<commit_message>
StateMachine 绑定 Animation 名称 &&  Animation 名称进行 Mix 匹配
</commit_message>
<xml_diff>
--- a/Config/Datas/ModelData.xlsx
+++ b/Config/Datas/ModelData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10511"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wantdabo\Documents\GitHub\goblin\Config\Datas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/goho/Documents/GitHub/goblin/Config/Datas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E053D58-1929-46F9-8E88-16D8F2E91BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F562BA-BF8A-9B4C-BDD4-0E196F080DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1440" yWindow="1960" windowWidth="28800" windowHeight="15340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ModelInfo" sheetId="1" r:id="rId1"/>
@@ -56,10 +56,12 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>AnimationMix</t>
-  </si>
-  <si>
-    <t>动画混合路径</t>
+    <t>Animation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>动画路径</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -70,7 +72,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -83,7 +85,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -479,12 +481,12 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="13.140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="26.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">

</xml_diff>